<commit_message>
box, colors, and font sizes
</commit_message>
<xml_diff>
--- a/Week of July 9 2023/Day 1/Attendance Tracker.xlsx
+++ b/Week of July 9 2023/Day 1/Attendance Tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbriody/Desktop/Coding Temple/Data-Analytics-Projects/Week of July 9 2023/Day 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FFBECD-3E35-8E47-9402-583FD36E4E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E26E8E-7A54-8B4B-9E4F-B246F2684482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{3E4B7A29-3A18-9B47-8AF0-A2A901AA8D72}"/>
   </bookViews>
@@ -317,7 +317,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -325,11 +325,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -339,13 +419,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -356,10 +432,24 @@
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -677,7 +767,7 @@
   <dimension ref="A1:Z48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="Q40" sqref="Q40"/>
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -698,64 +788,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
+      <c r="A1" s="23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
     </row>
     <row r="2" spans="1:26" ht="21" x14ac:dyDescent="0.25">
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="14" t="s">
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="5"/>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="20" t="s">
+      <c r="E3" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="20" t="s">
         <v>47</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
-      <c r="J3" s="16" t="s">
+      <c r="J3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="18" t="s">
+      <c r="K3" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="L3" s="20" t="s">
+      <c r="L3" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="M3" s="22" t="s">
+      <c r="M3" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="N3" s="24" t="s">
+      <c r="N3" s="20" t="s">
         <v>47</v>
       </c>
       <c r="O3" s="4"/>
@@ -776,39 +866,39 @@
         <v>2</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="17">
+      <c r="C4" s="13">
         <v>180</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="15">
         <f>180-C4</f>
         <v>0</v>
       </c>
-      <c r="E4" s="21">
+      <c r="E4" s="17">
         <v>5</v>
       </c>
-      <c r="F4" s="23">
+      <c r="F4" s="19">
         <f t="shared" ref="F4:F42" si="0">(C4-D4)/180</f>
         <v>1</v>
       </c>
-      <c r="G4" s="25">
+      <c r="G4" s="21">
         <f t="shared" ref="G4:G42" si="1">E4/C4</f>
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J4" s="13">
         <v>177</v>
       </c>
-      <c r="K4" s="19">
+      <c r="K4" s="15">
         <f>180-J4</f>
         <v>3</v>
       </c>
-      <c r="L4" s="21">
-        <v>2</v>
-      </c>
-      <c r="M4" s="23">
+      <c r="L4" s="17">
+        <v>2</v>
+      </c>
+      <c r="M4" s="19">
         <f>(J4-K4)/180</f>
         <v>0.96666666666666667</v>
       </c>
-      <c r="N4" s="25">
+      <c r="N4" s="21">
         <f>L4/J4</f>
         <v>1.1299435028248588E-2</v>
       </c>
@@ -818,39 +908,39 @@
         <v>3</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="17">
+      <c r="C5" s="13">
         <v>153</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="15">
         <f t="shared" ref="D5:D42" si="2">180-C5</f>
         <v>27</v>
       </c>
-      <c r="E5" s="21">
+      <c r="E5" s="17">
         <v>3</v>
       </c>
-      <c r="F5" s="23">
+      <c r="F5" s="19">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="G5" s="25">
+      <c r="G5" s="21">
         <f t="shared" si="1"/>
         <v>1.9607843137254902E-2</v>
       </c>
-      <c r="J5" s="17">
+      <c r="J5" s="13">
         <v>179</v>
       </c>
-      <c r="K5" s="19">
+      <c r="K5" s="15">
         <f t="shared" ref="K5:K42" si="3">180-J5</f>
         <v>1</v>
       </c>
-      <c r="L5" s="21">
+      <c r="L5" s="17">
         <v>4</v>
       </c>
-      <c r="M5" s="23">
+      <c r="M5" s="19">
         <f t="shared" ref="M5:M42" si="4">(J5-K5)/180</f>
         <v>0.98888888888888893</v>
       </c>
-      <c r="N5" s="25">
+      <c r="N5" s="21">
         <f t="shared" ref="N5:N42" si="5">L5/J5</f>
         <v>2.23463687150838E-2</v>
       </c>
@@ -860,39 +950,39 @@
         <v>4</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="17">
+      <c r="C6" s="13">
         <v>176</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="15">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="E6" s="21">
+      <c r="E6" s="17">
         <v>3</v>
       </c>
-      <c r="F6" s="23">
+      <c r="F6" s="19">
         <f t="shared" si="0"/>
         <v>0.9555555555555556</v>
       </c>
-      <c r="G6" s="25">
+      <c r="G6" s="21">
         <f t="shared" si="1"/>
         <v>1.7045454545454544E-2</v>
       </c>
-      <c r="J6" s="17">
+      <c r="J6" s="13">
         <v>174</v>
       </c>
-      <c r="K6" s="19">
+      <c r="K6" s="15">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="L6" s="21">
+      <c r="L6" s="17">
         <v>4</v>
       </c>
-      <c r="M6" s="23">
+      <c r="M6" s="19">
         <f t="shared" si="4"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="N6" s="25">
+      <c r="N6" s="21">
         <f t="shared" si="5"/>
         <v>2.2988505747126436E-2</v>
       </c>
@@ -902,39 +992,39 @@
         <v>5</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="17">
+      <c r="C7" s="13">
         <v>178</v>
       </c>
-      <c r="D7" s="19">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="E7" s="21">
-        <v>0</v>
-      </c>
-      <c r="F7" s="23">
+      <c r="D7" s="15">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E7" s="17">
+        <v>0</v>
+      </c>
+      <c r="F7" s="19">
         <f t="shared" si="0"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="G7" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J7" s="17">
+      <c r="G7" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="13">
         <v>180</v>
       </c>
-      <c r="K7" s="19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L7" s="21">
-        <v>2</v>
-      </c>
-      <c r="M7" s="23">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="N7" s="25">
+      <c r="K7" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="17">
+        <v>2</v>
+      </c>
+      <c r="M7" s="19">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N7" s="21">
         <f t="shared" si="5"/>
         <v>1.1111111111111112E-2</v>
       </c>
@@ -944,39 +1034,39 @@
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="17">
+      <c r="C8" s="13">
         <v>179</v>
       </c>
-      <c r="D8" s="19">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E8" s="21">
-        <v>2</v>
-      </c>
-      <c r="F8" s="23">
+      <c r="D8" s="15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="17">
+        <v>2</v>
+      </c>
+      <c r="F8" s="19">
         <f t="shared" si="0"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="G8" s="25">
+      <c r="G8" s="21">
         <f t="shared" si="1"/>
         <v>1.11731843575419E-2</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="13">
         <v>174</v>
       </c>
-      <c r="K8" s="19">
+      <c r="K8" s="15">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="L8" s="21">
+      <c r="L8" s="17">
         <v>4</v>
       </c>
-      <c r="M8" s="23">
+      <c r="M8" s="19">
         <f t="shared" si="4"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="N8" s="25">
+      <c r="N8" s="21">
         <f t="shared" si="5"/>
         <v>2.2988505747126436E-2</v>
       </c>
@@ -986,39 +1076,39 @@
         <v>7</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="17">
+      <c r="C9" s="13">
         <v>180</v>
       </c>
-      <c r="D9" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="21">
-        <v>1</v>
-      </c>
-      <c r="F9" s="23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G9" s="25">
+      <c r="D9" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="17">
+        <v>1</v>
+      </c>
+      <c r="F9" s="19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G9" s="21">
         <f t="shared" si="1"/>
         <v>5.5555555555555558E-3</v>
       </c>
-      <c r="J9" s="17">
+      <c r="J9" s="13">
         <v>178</v>
       </c>
-      <c r="K9" s="19">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L9" s="21">
-        <v>2</v>
-      </c>
-      <c r="M9" s="23">
+      <c r="K9" s="15">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L9" s="17">
+        <v>2</v>
+      </c>
+      <c r="M9" s="19">
         <f t="shared" si="4"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="N9" s="25">
+      <c r="N9" s="21">
         <f t="shared" si="5"/>
         <v>1.1235955056179775E-2</v>
       </c>
@@ -1028,39 +1118,39 @@
         <v>8</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="17">
+      <c r="C10" s="13">
         <v>168</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="15">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="E10" s="21">
-        <v>2</v>
-      </c>
-      <c r="F10" s="23">
+      <c r="E10" s="17">
+        <v>2</v>
+      </c>
+      <c r="F10" s="19">
         <f t="shared" si="0"/>
         <v>0.8666666666666667</v>
       </c>
-      <c r="G10" s="25">
+      <c r="G10" s="21">
         <f t="shared" si="1"/>
         <v>1.1904761904761904E-2</v>
       </c>
-      <c r="J10" s="17">
+      <c r="J10" s="13">
         <v>179</v>
       </c>
-      <c r="K10" s="19">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L10" s="21">
-        <v>1</v>
-      </c>
-      <c r="M10" s="23">
+      <c r="K10" s="15">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L10" s="17">
+        <v>1</v>
+      </c>
+      <c r="M10" s="19">
         <f t="shared" si="4"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="N10" s="25">
+      <c r="N10" s="21">
         <f t="shared" si="5"/>
         <v>5.5865921787709499E-3</v>
       </c>
@@ -1070,39 +1160,39 @@
         <v>9</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="17">
+      <c r="C11" s="13">
         <v>178</v>
       </c>
-      <c r="D11" s="19">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="E11" s="21">
+      <c r="D11" s="15">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E11" s="17">
         <v>15</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="19">
         <f t="shared" si="0"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="G11" s="25">
+      <c r="G11" s="21">
         <f t="shared" si="1"/>
         <v>8.4269662921348312E-2</v>
       </c>
-      <c r="J11" s="17">
+      <c r="J11" s="13">
         <v>177</v>
       </c>
-      <c r="K11" s="19">
+      <c r="K11" s="15">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="L11" s="21">
-        <v>0</v>
-      </c>
-      <c r="M11" s="23">
+      <c r="L11" s="17">
+        <v>0</v>
+      </c>
+      <c r="M11" s="19">
         <f t="shared" si="4"/>
         <v>0.96666666666666667</v>
       </c>
-      <c r="N11" s="25">
+      <c r="N11" s="21">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1112,39 +1202,39 @@
         <v>10</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="17">
+      <c r="C12" s="13">
         <v>174</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="15">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="E12" s="21">
-        <v>2</v>
-      </c>
-      <c r="F12" s="23">
+      <c r="E12" s="17">
+        <v>2</v>
+      </c>
+      <c r="F12" s="19">
         <f t="shared" si="0"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="G12" s="25">
+      <c r="G12" s="21">
         <f t="shared" si="1"/>
         <v>1.1494252873563218E-2</v>
       </c>
-      <c r="J12" s="17">
+      <c r="J12" s="13">
         <v>180</v>
       </c>
-      <c r="K12" s="19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L12" s="21">
+      <c r="K12" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="17">
         <v>6</v>
       </c>
-      <c r="M12" s="23">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="N12" s="25">
+      <c r="M12" s="19">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N12" s="21">
         <f t="shared" si="5"/>
         <v>3.3333333333333333E-2</v>
       </c>
@@ -1154,39 +1244,39 @@
         <v>11</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="17">
+      <c r="C13" s="13">
         <v>180</v>
       </c>
-      <c r="D13" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="21">
-        <v>1</v>
-      </c>
-      <c r="F13" s="23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G13" s="25">
+      <c r="D13" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="17">
+        <v>1</v>
+      </c>
+      <c r="F13" s="19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G13" s="21">
         <f t="shared" si="1"/>
         <v>5.5555555555555558E-3</v>
       </c>
-      <c r="J13" s="17">
+      <c r="J13" s="13">
         <v>176</v>
       </c>
-      <c r="K13" s="19">
+      <c r="K13" s="15">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="L13" s="21">
+      <c r="L13" s="17">
         <v>3</v>
       </c>
-      <c r="M13" s="23">
+      <c r="M13" s="19">
         <f t="shared" si="4"/>
         <v>0.9555555555555556</v>
       </c>
-      <c r="N13" s="25">
+      <c r="N13" s="21">
         <f t="shared" si="5"/>
         <v>1.7045454545454544E-2</v>
       </c>
@@ -1196,39 +1286,39 @@
         <v>12</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="17">
+      <c r="C14" s="13">
         <v>174</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="15">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="E14" s="21">
-        <v>0</v>
-      </c>
-      <c r="F14" s="23">
+      <c r="E14" s="17">
+        <v>0</v>
+      </c>
+      <c r="F14" s="19">
         <f t="shared" si="0"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="G14" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="17">
+      <c r="G14" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="13">
         <v>174</v>
       </c>
-      <c r="K14" s="19">
+      <c r="K14" s="15">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="L14" s="21">
+      <c r="L14" s="17">
         <v>5</v>
       </c>
-      <c r="M14" s="23">
+      <c r="M14" s="19">
         <f t="shared" si="4"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="N14" s="25">
+      <c r="N14" s="21">
         <f t="shared" si="5"/>
         <v>2.8735632183908046E-2</v>
       </c>
@@ -1238,39 +1328,39 @@
         <v>13</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="17">
+      <c r="C15" s="13">
         <v>179</v>
       </c>
-      <c r="D15" s="19">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E15" s="21">
-        <v>2</v>
-      </c>
-      <c r="F15" s="23">
+      <c r="D15" s="15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="17">
+        <v>2</v>
+      </c>
+      <c r="F15" s="19">
         <f t="shared" si="0"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="G15" s="25">
+      <c r="G15" s="21">
         <f t="shared" si="1"/>
         <v>1.11731843575419E-2</v>
       </c>
-      <c r="J15" s="17">
+      <c r="J15" s="13">
         <v>178</v>
       </c>
-      <c r="K15" s="19">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L15" s="21">
+      <c r="K15" s="15">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L15" s="17">
         <v>3</v>
       </c>
-      <c r="M15" s="23">
+      <c r="M15" s="19">
         <f t="shared" si="4"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="N15" s="25">
+      <c r="N15" s="21">
         <f t="shared" si="5"/>
         <v>1.6853932584269662E-2</v>
       </c>
@@ -1280,39 +1370,39 @@
         <v>14</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="17">
+      <c r="C16" s="13">
         <v>176</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="15">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="E16" s="21">
+      <c r="E16" s="17">
         <v>5</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="19">
         <f t="shared" si="0"/>
         <v>0.9555555555555556</v>
       </c>
-      <c r="G16" s="25">
+      <c r="G16" s="21">
         <f t="shared" si="1"/>
         <v>2.8409090909090908E-2</v>
       </c>
-      <c r="J16" s="17">
+      <c r="J16" s="13">
         <v>179</v>
       </c>
-      <c r="K16" s="19">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L16" s="21">
-        <v>2</v>
-      </c>
-      <c r="M16" s="23">
+      <c r="K16" s="15">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L16" s="17">
+        <v>2</v>
+      </c>
+      <c r="M16" s="19">
         <f t="shared" si="4"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="N16" s="25">
+      <c r="N16" s="21">
         <f t="shared" si="5"/>
         <v>1.11731843575419E-2</v>
       </c>
@@ -1322,39 +1412,39 @@
         <v>15</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="17">
+      <c r="C17" s="13">
         <v>178</v>
       </c>
-      <c r="D17" s="19">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="E17" s="21">
-        <v>0</v>
-      </c>
-      <c r="F17" s="23">
+      <c r="D17" s="15">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E17" s="17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="19">
         <f t="shared" si="0"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="G17" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="17">
+      <c r="G17" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="13">
         <v>178</v>
       </c>
-      <c r="K17" s="19">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L17" s="21">
-        <v>0</v>
-      </c>
-      <c r="M17" s="23">
+      <c r="K17" s="15">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L17" s="17">
+        <v>0</v>
+      </c>
+      <c r="M17" s="19">
         <f t="shared" si="4"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="N17" s="25">
+      <c r="N17" s="21">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1364,39 +1454,39 @@
         <v>16</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="17">
+      <c r="C18" s="13">
         <v>177</v>
       </c>
-      <c r="D18" s="19">
+      <c r="D18" s="15">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="17">
         <v>4</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18" s="19">
         <f t="shared" si="0"/>
         <v>0.96666666666666667</v>
       </c>
-      <c r="G18" s="25">
+      <c r="G18" s="21">
         <f t="shared" si="1"/>
         <v>2.2598870056497175E-2</v>
       </c>
-      <c r="J18" s="17">
+      <c r="J18" s="13">
         <v>174</v>
       </c>
-      <c r="K18" s="19">
+      <c r="K18" s="15">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="L18" s="21">
+      <c r="L18" s="17">
         <v>5</v>
       </c>
-      <c r="M18" s="23">
+      <c r="M18" s="19">
         <f t="shared" si="4"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="N18" s="25">
+      <c r="N18" s="21">
         <f t="shared" si="5"/>
         <v>2.8735632183908046E-2</v>
       </c>
@@ -1406,39 +1496,39 @@
         <v>17</v>
       </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="17">
+      <c r="C19" s="13">
         <v>180</v>
       </c>
-      <c r="D19" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="21">
-        <v>2</v>
-      </c>
-      <c r="F19" s="23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G19" s="25">
+      <c r="D19" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="17">
+        <v>2</v>
+      </c>
+      <c r="F19" s="19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G19" s="21">
         <f t="shared" si="1"/>
         <v>1.1111111111111112E-2</v>
       </c>
-      <c r="J19" s="17">
+      <c r="J19" s="13">
         <v>177</v>
       </c>
-      <c r="K19" s="19">
+      <c r="K19" s="15">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="L19" s="21">
+      <c r="L19" s="17">
         <v>6</v>
       </c>
-      <c r="M19" s="23">
+      <c r="M19" s="19">
         <f t="shared" si="4"/>
         <v>0.96666666666666667</v>
       </c>
-      <c r="N19" s="25">
+      <c r="N19" s="21">
         <f t="shared" si="5"/>
         <v>3.3898305084745763E-2</v>
       </c>
@@ -1448,39 +1538,39 @@
         <v>18</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="17">
+      <c r="C20" s="13">
         <v>172</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="15">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="E20" s="21">
-        <v>0</v>
-      </c>
-      <c r="F20" s="23">
+      <c r="E20" s="17">
+        <v>0</v>
+      </c>
+      <c r="F20" s="19">
         <f t="shared" si="0"/>
         <v>0.91111111111111109</v>
       </c>
-      <c r="G20" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="17">
+      <c r="G20" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="13">
         <v>178</v>
       </c>
-      <c r="K20" s="19">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L20" s="21">
-        <v>2</v>
-      </c>
-      <c r="M20" s="23">
+      <c r="K20" s="15">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L20" s="17">
+        <v>2</v>
+      </c>
+      <c r="M20" s="19">
         <f t="shared" si="4"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="N20" s="25">
+      <c r="N20" s="21">
         <f t="shared" si="5"/>
         <v>1.1235955056179775E-2</v>
       </c>
@@ -1490,39 +1580,39 @@
         <v>19</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="17">
+      <c r="C21" s="13">
         <v>178</v>
       </c>
-      <c r="D21" s="19">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="E21" s="21">
+      <c r="D21" s="15">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E21" s="17">
         <v>5</v>
       </c>
-      <c r="F21" s="23">
+      <c r="F21" s="19">
         <f t="shared" si="0"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="G21" s="25">
+      <c r="G21" s="21">
         <f t="shared" si="1"/>
         <v>2.8089887640449437E-2</v>
       </c>
-      <c r="J21" s="17">
+      <c r="J21" s="13">
         <v>169</v>
       </c>
-      <c r="K21" s="19">
+      <c r="K21" s="15">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="L21" s="21">
+      <c r="L21" s="17">
         <v>3</v>
       </c>
-      <c r="M21" s="23">
+      <c r="M21" s="19">
         <f t="shared" si="4"/>
         <v>0.87777777777777777</v>
       </c>
-      <c r="N21" s="25">
+      <c r="N21" s="21">
         <f t="shared" si="5"/>
         <v>1.7751479289940829E-2</v>
       </c>
@@ -1532,39 +1622,39 @@
         <v>20</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="17">
+      <c r="C22" s="13">
         <v>172</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="15">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="E22" s="21">
-        <v>2</v>
-      </c>
-      <c r="F22" s="23">
+      <c r="E22" s="17">
+        <v>2</v>
+      </c>
+      <c r="F22" s="19">
         <f t="shared" si="0"/>
         <v>0.91111111111111109</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22" s="21">
         <f t="shared" si="1"/>
         <v>1.1627906976744186E-2</v>
       </c>
-      <c r="J22" s="17">
+      <c r="J22" s="13">
         <v>177</v>
       </c>
-      <c r="K22" s="19">
+      <c r="K22" s="15">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="L22" s="21">
+      <c r="L22" s="17">
         <v>16</v>
       </c>
-      <c r="M22" s="23">
+      <c r="M22" s="19">
         <f t="shared" si="4"/>
         <v>0.96666666666666667</v>
       </c>
-      <c r="N22" s="25">
+      <c r="N22" s="21">
         <f t="shared" si="5"/>
         <v>9.03954802259887E-2</v>
       </c>
@@ -1574,39 +1664,39 @@
         <v>21</v>
       </c>
       <c r="B23" s="2"/>
-      <c r="C23" s="17">
+      <c r="C23" s="13">
         <v>178</v>
       </c>
-      <c r="D23" s="19">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="E23" s="21">
-        <v>2</v>
-      </c>
-      <c r="F23" s="23">
+      <c r="D23" s="15">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E23" s="17">
+        <v>2</v>
+      </c>
+      <c r="F23" s="19">
         <f t="shared" si="0"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="G23" s="25">
+      <c r="G23" s="21">
         <f t="shared" si="1"/>
         <v>1.1235955056179775E-2</v>
       </c>
-      <c r="J23" s="17">
+      <c r="J23" s="13">
         <v>179</v>
       </c>
-      <c r="K23" s="19">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L23" s="21">
-        <v>2</v>
-      </c>
-      <c r="M23" s="23">
+      <c r="K23" s="15">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L23" s="17">
+        <v>2</v>
+      </c>
+      <c r="M23" s="19">
         <f t="shared" si="4"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="N23" s="25">
+      <c r="N23" s="21">
         <f t="shared" si="5"/>
         <v>1.11731843575419E-2</v>
       </c>
@@ -1616,39 +1706,39 @@
         <v>22</v>
       </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="17">
+      <c r="C24" s="13">
         <v>174</v>
       </c>
-      <c r="D24" s="19">
+      <c r="D24" s="15">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="E24" s="21">
-        <v>0</v>
-      </c>
-      <c r="F24" s="23">
+      <c r="E24" s="17">
+        <v>0</v>
+      </c>
+      <c r="F24" s="19">
         <f t="shared" si="0"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="G24" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J24" s="17">
+      <c r="G24" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="13">
         <v>180</v>
       </c>
-      <c r="K24" s="19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L24" s="21">
+      <c r="K24" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="17">
         <v>5</v>
       </c>
-      <c r="M24" s="23">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="N24" s="25">
+      <c r="M24" s="19">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N24" s="21">
         <f t="shared" si="5"/>
         <v>2.7777777777777776E-2</v>
       </c>
@@ -1658,39 +1748,39 @@
         <v>23</v>
       </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="17">
+      <c r="C25" s="13">
         <v>179</v>
       </c>
-      <c r="D25" s="19">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E25" s="21">
+      <c r="D25" s="15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E25" s="17">
         <v>6</v>
       </c>
-      <c r="F25" s="23">
+      <c r="F25" s="19">
         <f t="shared" si="0"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="G25" s="25">
+      <c r="G25" s="21">
         <f t="shared" si="1"/>
         <v>3.3519553072625698E-2</v>
       </c>
-      <c r="J25" s="17">
+      <c r="J25" s="13">
         <v>176</v>
       </c>
-      <c r="K25" s="19">
+      <c r="K25" s="15">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="L25" s="21">
-        <v>0</v>
-      </c>
-      <c r="M25" s="23">
+      <c r="L25" s="17">
+        <v>0</v>
+      </c>
+      <c r="M25" s="19">
         <f t="shared" si="4"/>
         <v>0.9555555555555556</v>
       </c>
-      <c r="N25" s="25">
+      <c r="N25" s="21">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1700,39 +1790,39 @@
         <v>24</v>
       </c>
       <c r="B26" s="2"/>
-      <c r="C26" s="17">
+      <c r="C26" s="13">
         <v>174</v>
       </c>
-      <c r="D26" s="19">
+      <c r="D26" s="15">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="E26" s="21">
+      <c r="E26" s="17">
         <v>13</v>
       </c>
-      <c r="F26" s="23">
+      <c r="F26" s="19">
         <f t="shared" si="0"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="G26" s="25">
+      <c r="G26" s="21">
         <f t="shared" si="1"/>
         <v>7.4712643678160925E-2</v>
       </c>
-      <c r="J26" s="17">
+      <c r="J26" s="13">
         <v>172</v>
       </c>
-      <c r="K26" s="19">
+      <c r="K26" s="15">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="L26" s="21">
-        <v>2</v>
-      </c>
-      <c r="M26" s="23">
+      <c r="L26" s="17">
+        <v>2</v>
+      </c>
+      <c r="M26" s="19">
         <f t="shared" si="4"/>
         <v>0.91111111111111109</v>
       </c>
-      <c r="N26" s="25">
+      <c r="N26" s="21">
         <f t="shared" si="5"/>
         <v>1.1627906976744186E-2</v>
       </c>
@@ -1742,39 +1832,39 @@
         <v>35</v>
       </c>
       <c r="B27" s="2"/>
-      <c r="C27" s="17">
+      <c r="C27" s="13">
         <v>180</v>
       </c>
-      <c r="D27" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E27" s="21">
-        <v>2</v>
-      </c>
-      <c r="F27" s="23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G27" s="25">
+      <c r="D27" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="17">
+        <v>2</v>
+      </c>
+      <c r="F27" s="19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G27" s="21">
         <f t="shared" si="1"/>
         <v>1.1111111111111112E-2</v>
       </c>
-      <c r="J27" s="17">
+      <c r="J27" s="13">
         <v>179</v>
       </c>
-      <c r="K27" s="19">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L27" s="21">
+      <c r="K27" s="15">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L27" s="17">
         <v>6</v>
       </c>
-      <c r="M27" s="23">
+      <c r="M27" s="19">
         <f t="shared" si="4"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="N27" s="25">
+      <c r="N27" s="21">
         <f t="shared" si="5"/>
         <v>3.3519553072625698E-2</v>
       </c>
@@ -1784,39 +1874,39 @@
         <v>25</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="17">
+      <c r="C28" s="13">
         <v>177</v>
       </c>
-      <c r="D28" s="19">
+      <c r="D28" s="15">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="E28" s="21">
+      <c r="E28" s="17">
         <v>4</v>
       </c>
-      <c r="F28" s="23">
+      <c r="F28" s="19">
         <f t="shared" si="0"/>
         <v>0.96666666666666667</v>
       </c>
-      <c r="G28" s="25">
+      <c r="G28" s="21">
         <f t="shared" si="1"/>
         <v>2.2598870056497175E-2</v>
       </c>
-      <c r="J28" s="17">
+      <c r="J28" s="13">
         <v>178</v>
       </c>
-      <c r="K28" s="19">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L28" s="21">
+      <c r="K28" s="15">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L28" s="17">
         <v>4</v>
       </c>
-      <c r="M28" s="23">
+      <c r="M28" s="19">
         <f t="shared" si="4"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="N28" s="25">
+      <c r="N28" s="21">
         <f t="shared" si="5"/>
         <v>2.247191011235955E-2</v>
       </c>
@@ -1826,39 +1916,39 @@
         <v>26</v>
       </c>
       <c r="B29" s="2"/>
-      <c r="C29" s="17">
+      <c r="C29" s="13">
         <v>176</v>
       </c>
-      <c r="D29" s="19">
+      <c r="D29" s="15">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="E29" s="21">
-        <v>0</v>
-      </c>
-      <c r="F29" s="23">
+      <c r="E29" s="17">
+        <v>0</v>
+      </c>
+      <c r="F29" s="19">
         <f t="shared" si="0"/>
         <v>0.9555555555555556</v>
       </c>
-      <c r="G29" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J29" s="17">
+      <c r="G29" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="13">
         <v>177</v>
       </c>
-      <c r="K29" s="19">
+      <c r="K29" s="15">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="L29" s="21">
-        <v>2</v>
-      </c>
-      <c r="M29" s="23">
+      <c r="L29" s="17">
+        <v>2</v>
+      </c>
+      <c r="M29" s="19">
         <f t="shared" si="4"/>
         <v>0.96666666666666667</v>
       </c>
-      <c r="N29" s="25">
+      <c r="N29" s="21">
         <f t="shared" si="5"/>
         <v>1.1299435028248588E-2</v>
       </c>
@@ -1868,39 +1958,39 @@
         <v>27</v>
       </c>
       <c r="B30" s="2"/>
-      <c r="C30" s="17">
+      <c r="C30" s="13">
         <v>180</v>
       </c>
-      <c r="D30" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E30" s="21">
+      <c r="D30" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="17">
         <v>5</v>
       </c>
-      <c r="F30" s="23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G30" s="25">
+      <c r="F30" s="19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G30" s="21">
         <f t="shared" si="1"/>
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="J30" s="17">
+      <c r="J30" s="13">
         <v>180</v>
       </c>
-      <c r="K30" s="19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L30" s="21">
+      <c r="K30" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="17">
         <v>6</v>
       </c>
-      <c r="M30" s="23">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="N30" s="25">
+      <c r="M30" s="19">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N30" s="21">
         <f t="shared" si="5"/>
         <v>3.3333333333333333E-2</v>
       </c>
@@ -1910,39 +2000,39 @@
         <v>28</v>
       </c>
       <c r="B31" s="2"/>
-      <c r="C31" s="17">
+      <c r="C31" s="13">
         <v>174</v>
       </c>
-      <c r="D31" s="19">
+      <c r="D31" s="15">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="E31" s="21">
+      <c r="E31" s="17">
         <v>5</v>
       </c>
-      <c r="F31" s="23">
+      <c r="F31" s="19">
         <f t="shared" si="0"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="G31" s="25">
+      <c r="G31" s="21">
         <f t="shared" si="1"/>
         <v>2.8735632183908046E-2</v>
       </c>
-      <c r="J31" s="17">
+      <c r="J31" s="13">
         <v>177</v>
       </c>
-      <c r="K31" s="19">
+      <c r="K31" s="15">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="L31" s="21">
-        <v>2</v>
-      </c>
-      <c r="M31" s="23">
+      <c r="L31" s="17">
+        <v>2</v>
+      </c>
+      <c r="M31" s="19">
         <f t="shared" si="4"/>
         <v>0.96666666666666667</v>
       </c>
-      <c r="N31" s="25">
+      <c r="N31" s="21">
         <f t="shared" si="5"/>
         <v>1.1299435028248588E-2</v>
       </c>
@@ -1952,39 +2042,39 @@
         <v>29</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="17">
+      <c r="C32" s="13">
         <v>177</v>
       </c>
-      <c r="D32" s="19">
+      <c r="D32" s="15">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="E32" s="21">
-        <v>2</v>
-      </c>
-      <c r="F32" s="23">
+      <c r="E32" s="17">
+        <v>2</v>
+      </c>
+      <c r="F32" s="19">
         <f t="shared" si="0"/>
         <v>0.96666666666666667</v>
       </c>
-      <c r="G32" s="25">
+      <c r="G32" s="21">
         <f t="shared" si="1"/>
         <v>1.1299435028248588E-2</v>
       </c>
-      <c r="J32" s="17">
+      <c r="J32" s="13">
         <v>172</v>
       </c>
-      <c r="K32" s="19">
+      <c r="K32" s="15">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="L32" s="21">
+      <c r="L32" s="17">
         <v>4</v>
       </c>
-      <c r="M32" s="23">
+      <c r="M32" s="19">
         <f t="shared" si="4"/>
         <v>0.91111111111111109</v>
       </c>
-      <c r="N32" s="25">
+      <c r="N32" s="21">
         <f t="shared" si="5"/>
         <v>2.3255813953488372E-2</v>
       </c>
@@ -1994,39 +2084,39 @@
         <v>36</v>
       </c>
       <c r="B33" s="2"/>
-      <c r="C33" s="17">
+      <c r="C33" s="13">
         <v>180</v>
       </c>
-      <c r="D33" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E33" s="21">
-        <v>0</v>
-      </c>
-      <c r="F33" s="23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G33" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J33" s="17">
+      <c r="D33" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="17">
+        <v>0</v>
+      </c>
+      <c r="F33" s="19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G33" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="13">
         <v>178</v>
       </c>
-      <c r="K33" s="19">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L33" s="21">
+      <c r="K33" s="15">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L33" s="17">
         <v>4</v>
       </c>
-      <c r="M33" s="23">
+      <c r="M33" s="19">
         <f t="shared" si="4"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="N33" s="25">
+      <c r="N33" s="21">
         <f t="shared" si="5"/>
         <v>2.247191011235955E-2</v>
       </c>
@@ -2036,39 +2126,39 @@
         <v>37</v>
       </c>
       <c r="B34" s="2"/>
-      <c r="C34" s="17">
+      <c r="C34" s="13">
         <v>174</v>
       </c>
-      <c r="D34" s="19">
+      <c r="D34" s="15">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="E34" s="21">
-        <v>2</v>
-      </c>
-      <c r="F34" s="23">
+      <c r="E34" s="17">
+        <v>2</v>
+      </c>
+      <c r="F34" s="19">
         <f t="shared" si="0"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="G34" s="25">
+      <c r="G34" s="21">
         <f t="shared" si="1"/>
         <v>1.1494252873563218E-2</v>
       </c>
-      <c r="J34" s="17">
+      <c r="J34" s="13">
         <v>178</v>
       </c>
-      <c r="K34" s="19">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L34" s="21">
-        <v>1</v>
-      </c>
-      <c r="M34" s="23">
+      <c r="K34" s="15">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L34" s="17">
+        <v>1</v>
+      </c>
+      <c r="M34" s="19">
         <f t="shared" si="4"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="N34" s="25">
+      <c r="N34" s="21">
         <f t="shared" si="5"/>
         <v>5.6179775280898875E-3</v>
       </c>
@@ -2078,39 +2168,39 @@
         <v>38</v>
       </c>
       <c r="B35" s="2"/>
-      <c r="C35" s="17">
+      <c r="C35" s="13">
         <v>179</v>
       </c>
-      <c r="D35" s="19">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E35" s="21">
-        <v>1</v>
-      </c>
-      <c r="F35" s="23">
+      <c r="D35" s="15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E35" s="17">
+        <v>1</v>
+      </c>
+      <c r="F35" s="19">
         <f t="shared" si="0"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="G35" s="25">
+      <c r="G35" s="21">
         <f t="shared" si="1"/>
         <v>5.5865921787709499E-3</v>
       </c>
-      <c r="J35" s="17">
+      <c r="J35" s="13">
         <v>179</v>
       </c>
-      <c r="K35" s="19">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L35" s="21">
-        <v>0</v>
-      </c>
-      <c r="M35" s="23">
+      <c r="K35" s="15">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L35" s="17">
+        <v>0</v>
+      </c>
+      <c r="M35" s="19">
         <f t="shared" si="4"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="N35" s="25">
+      <c r="N35" s="21">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2120,39 +2210,39 @@
         <v>30</v>
       </c>
       <c r="B36" s="2"/>
-      <c r="C36" s="17">
+      <c r="C36" s="13">
         <v>180</v>
       </c>
-      <c r="D36" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E36" s="21">
+      <c r="D36" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E36" s="17">
         <v>3</v>
       </c>
-      <c r="F36" s="23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G36" s="25">
+      <c r="F36" s="19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G36" s="21">
         <f t="shared" si="1"/>
         <v>1.6666666666666666E-2</v>
       </c>
-      <c r="J36" s="17">
+      <c r="J36" s="13">
         <v>179</v>
       </c>
-      <c r="K36" s="19">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L36" s="21">
-        <v>2</v>
-      </c>
-      <c r="M36" s="23">
+      <c r="K36" s="15">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L36" s="17">
+        <v>2</v>
+      </c>
+      <c r="M36" s="19">
         <f t="shared" si="4"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="N36" s="25">
+      <c r="N36" s="21">
         <f t="shared" si="5"/>
         <v>1.11731843575419E-2</v>
       </c>
@@ -2162,39 +2252,39 @@
         <v>31</v>
       </c>
       <c r="B37" s="2"/>
-      <c r="C37" s="17">
+      <c r="C37" s="13">
         <v>174</v>
       </c>
-      <c r="D37" s="19">
+      <c r="D37" s="15">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="E37" s="21">
-        <v>0</v>
-      </c>
-      <c r="F37" s="23">
+      <c r="E37" s="17">
+        <v>0</v>
+      </c>
+      <c r="F37" s="19">
         <f t="shared" si="0"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="G37" s="25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J37" s="17">
+      <c r="G37" s="21">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="13">
         <v>180</v>
       </c>
-      <c r="K37" s="19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L37" s="21">
+      <c r="K37" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L37" s="17">
         <v>4</v>
       </c>
-      <c r="M37" s="23">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="N37" s="25">
+      <c r="M37" s="19">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N37" s="21">
         <f t="shared" si="5"/>
         <v>2.2222222222222223E-2</v>
       </c>
@@ -2204,39 +2294,39 @@
         <v>32</v>
       </c>
       <c r="B38" s="2"/>
-      <c r="C38" s="17">
+      <c r="C38" s="13">
         <v>178</v>
       </c>
-      <c r="D38" s="19">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="E38" s="21">
-        <v>2</v>
-      </c>
-      <c r="F38" s="23">
+      <c r="D38" s="15">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E38" s="17">
+        <v>2</v>
+      </c>
+      <c r="F38" s="19">
         <f t="shared" si="0"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="G38" s="25">
+      <c r="G38" s="21">
         <f t="shared" si="1"/>
         <v>1.1235955056179775E-2</v>
       </c>
-      <c r="J38" s="17">
+      <c r="J38" s="13">
         <v>174</v>
       </c>
-      <c r="K38" s="19">
+      <c r="K38" s="15">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="L38" s="21">
-        <v>0</v>
-      </c>
-      <c r="M38" s="23">
+      <c r="L38" s="17">
+        <v>0</v>
+      </c>
+      <c r="M38" s="19">
         <f t="shared" si="4"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="N38" s="25">
+      <c r="N38" s="21">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2246,39 +2336,39 @@
         <v>33</v>
       </c>
       <c r="B39" s="2"/>
-      <c r="C39" s="17">
+      <c r="C39" s="13">
         <v>172</v>
       </c>
-      <c r="D39" s="19">
+      <c r="D39" s="15">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="E39" s="21">
+      <c r="E39" s="17">
         <v>4</v>
       </c>
-      <c r="F39" s="23">
+      <c r="F39" s="19">
         <f t="shared" si="0"/>
         <v>0.91111111111111109</v>
       </c>
-      <c r="G39" s="25">
+      <c r="G39" s="21">
         <f t="shared" si="1"/>
         <v>2.3255813953488372E-2</v>
       </c>
-      <c r="J39" s="17">
+      <c r="J39" s="13">
         <v>177</v>
       </c>
-      <c r="K39" s="19">
+      <c r="K39" s="15">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="L39" s="21">
+      <c r="L39" s="17">
         <v>6</v>
       </c>
-      <c r="M39" s="23">
+      <c r="M39" s="19">
         <f t="shared" si="4"/>
         <v>0.96666666666666667</v>
       </c>
-      <c r="N39" s="25">
+      <c r="N39" s="21">
         <f t="shared" si="5"/>
         <v>3.3898305084745763E-2</v>
       </c>
@@ -2288,39 +2378,39 @@
         <v>34</v>
       </c>
       <c r="B40" s="2"/>
-      <c r="C40" s="17">
+      <c r="C40" s="13">
         <v>179</v>
       </c>
-      <c r="D40" s="19">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E40" s="21">
-        <v>1</v>
-      </c>
-      <c r="F40" s="23">
+      <c r="D40" s="15">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E40" s="17">
+        <v>1</v>
+      </c>
+      <c r="F40" s="19">
         <f t="shared" si="0"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="G40" s="25">
+      <c r="G40" s="21">
         <f t="shared" si="1"/>
         <v>5.5865921787709499E-3</v>
       </c>
-      <c r="J40" s="17">
+      <c r="J40" s="13">
         <v>180</v>
       </c>
-      <c r="K40" s="19">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L40" s="21">
-        <v>2</v>
-      </c>
-      <c r="M40" s="23">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="N40" s="25">
+      <c r="K40" s="15">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L40" s="17">
+        <v>2</v>
+      </c>
+      <c r="M40" s="19">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N40" s="21">
         <f t="shared" si="5"/>
         <v>1.1111111111111112E-2</v>
       </c>
@@ -2330,39 +2420,39 @@
         <v>39</v>
       </c>
       <c r="B41" s="2"/>
-      <c r="C41" s="17">
+      <c r="C41" s="13">
         <v>180</v>
       </c>
-      <c r="D41" s="19">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E41" s="21">
-        <v>2</v>
-      </c>
-      <c r="F41" s="23">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G41" s="25">
+      <c r="D41" s="15">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E41" s="17">
+        <v>2</v>
+      </c>
+      <c r="F41" s="19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G41" s="21">
         <f t="shared" si="1"/>
         <v>1.1111111111111112E-2</v>
       </c>
-      <c r="J41" s="17">
+      <c r="J41" s="13">
         <v>174</v>
       </c>
-      <c r="K41" s="19">
+      <c r="K41" s="15">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="L41" s="21">
+      <c r="L41" s="17">
         <v>5</v>
       </c>
-      <c r="M41" s="23">
+      <c r="M41" s="19">
         <f t="shared" si="4"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="N41" s="25">
+      <c r="N41" s="21">
         <f t="shared" si="5"/>
         <v>2.8735632183908046E-2</v>
       </c>
@@ -2372,185 +2462,189 @@
         <v>40</v>
       </c>
       <c r="B42" s="2"/>
-      <c r="C42" s="17">
+      <c r="C42" s="13">
         <v>177</v>
       </c>
-      <c r="D42" s="19">
+      <c r="D42" s="15">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="E42" s="21">
+      <c r="E42" s="17">
         <v>5</v>
       </c>
-      <c r="F42" s="23">
+      <c r="F42" s="19">
         <f t="shared" si="0"/>
         <v>0.96666666666666667</v>
       </c>
-      <c r="G42" s="25">
+      <c r="G42" s="21">
         <f t="shared" si="1"/>
         <v>2.8248587570621469E-2</v>
       </c>
-      <c r="J42" s="17">
+      <c r="J42" s="13">
         <v>170</v>
       </c>
-      <c r="K42" s="19">
+      <c r="K42" s="15">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="L42" s="21">
-        <v>1</v>
-      </c>
-      <c r="M42" s="23">
+      <c r="L42" s="17">
+        <v>1</v>
+      </c>
+      <c r="M42" s="19">
         <f t="shared" si="4"/>
         <v>0.88888888888888884</v>
       </c>
-      <c r="N42" s="25">
+      <c r="N42" s="21">
         <f t="shared" si="5"/>
         <v>5.8823529411764705E-3</v>
       </c>
     </row>
-    <row r="43" spans="1:14" ht="20" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" ht="21" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="F43" s="6"/>
       <c r="M43" s="6"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44" s="9" t="s">
+      <c r="A44" s="24" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="9"/>
-      <c r="C44">
+      <c r="B44" s="25"/>
+      <c r="C44" s="26">
         <f>MAX(C4:C42)</f>
         <v>180</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="26">
         <f>MAX(D4:D42)</f>
         <v>27</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="26">
         <f>MAX(E4:E42)</f>
         <v>15</v>
       </c>
-      <c r="F44" s="6">
+      <c r="F44" s="27">
         <f>MAX(F4:F42)</f>
         <v>1</v>
       </c>
-      <c r="G44" s="6">
+      <c r="G44" s="27">
         <f>MAX(G4:G42)</f>
         <v>8.4269662921348312E-2</v>
       </c>
-      <c r="J44">
+      <c r="H44" s="26"/>
+      <c r="I44" s="26"/>
+      <c r="J44" s="26">
         <f>MAX(J4:J42)</f>
         <v>180</v>
       </c>
-      <c r="K44">
+      <c r="K44" s="26">
         <f>MAX(K4:K42)</f>
         <v>11</v>
       </c>
-      <c r="L44">
+      <c r="L44" s="26">
         <f>MAX(L4:L42)</f>
         <v>16</v>
       </c>
-      <c r="M44" s="6">
+      <c r="M44" s="27">
         <f>MAX(M4:M42)</f>
         <v>1</v>
       </c>
-      <c r="N44" s="6">
+      <c r="N44" s="28">
         <f>MAX(N4:N42)</f>
         <v>9.03954802259887E-2</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45" s="10" t="s">
+      <c r="A45" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="10"/>
-      <c r="C45">
+      <c r="B45" s="30"/>
+      <c r="C45" s="31">
         <f>MIN(C4:C42)</f>
         <v>153</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="31">
         <f>MIN(D4:D42)</f>
         <v>0</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="31">
         <f>MIN(E4:E42)</f>
         <v>0</v>
       </c>
-      <c r="F45" s="6">
+      <c r="F45" s="32">
         <f>MIN(F4:F42)</f>
         <v>0.7</v>
       </c>
-      <c r="G45" s="6">
+      <c r="G45" s="32">
         <f>MIN(G4:G42)</f>
         <v>0</v>
       </c>
-      <c r="J45">
+      <c r="H45" s="31"/>
+      <c r="I45" s="31"/>
+      <c r="J45" s="31">
         <f>MIN(J4:J42)</f>
         <v>169</v>
       </c>
-      <c r="K45">
+      <c r="K45" s="31">
         <f>MIN(K4:K42)</f>
         <v>0</v>
       </c>
-      <c r="L45">
+      <c r="L45" s="31">
         <f>MIN(L4:L42)</f>
         <v>0</v>
       </c>
-      <c r="M45" s="6">
+      <c r="M45" s="32">
         <f>MIN(M4:M42)</f>
         <v>0.87777777777777777</v>
       </c>
-      <c r="N45" s="6">
+      <c r="N45" s="33">
         <f>MIN(N4:N42)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:14" ht="19" x14ac:dyDescent="0.25">
-      <c r="A46" s="26" t="s">
+    <row r="46" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="26"/>
-      <c r="C46" s="27">
+      <c r="B46" s="35"/>
+      <c r="C46" s="36">
         <f>AVERAGE(C4:C42)</f>
         <v>176.25641025641025</v>
       </c>
-      <c r="D46" s="27">
+      <c r="D46" s="36">
         <f>AVERAGE(D4:D42)</f>
         <v>3.7435897435897436</v>
       </c>
-      <c r="E46" s="27">
+      <c r="E46" s="36">
         <f>AVERAGE(E4:E42)</f>
         <v>2.8974358974358974</v>
       </c>
-      <c r="F46" s="28">
+      <c r="F46" s="37">
         <f>AVERAGE(F4:F42)</f>
         <v>0.95840455840455829</v>
       </c>
-      <c r="G46" s="28">
+      <c r="G46" s="37">
         <f>AVERAGE(G4:G42)</f>
         <v>1.6450529467536674E-2</v>
       </c>
-      <c r="H46" s="29"/>
-      <c r="I46" s="29"/>
-      <c r="J46" s="27">
+      <c r="H46" s="38"/>
+      <c r="I46" s="38"/>
+      <c r="J46" s="36">
         <f>AVERAGE(J4:J42)</f>
         <v>176.84615384615384</v>
       </c>
-      <c r="K46" s="27">
+      <c r="K46" s="36">
         <f>AVERAGE(K4:K42)</f>
         <v>3.1538461538461537</v>
       </c>
-      <c r="L46" s="27">
+      <c r="L46" s="36">
         <f>AVERAGE(L4:L42)</f>
         <v>3.2820512820512819</v>
       </c>
-      <c r="M46" s="28">
+      <c r="M46" s="37">
         <f>AVERAGE(M4:M42)</f>
         <v>0.96495726495726453</v>
       </c>
-      <c r="N46" s="28">
+      <c r="N46" s="39">
         <f>AVERAGE(N4:N42)</f>
         <v>1.8553484810524122E-2</v>
       </c>

</xml_diff>

<commit_message>
Grids for colored sections
</commit_message>
<xml_diff>
--- a/Week of July 9 2023/Day 1/Attendance Tracker.xlsx
+++ b/Week of July 9 2023/Day 1/Attendance Tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderbriody/Desktop/Coding Temple/Data-Analytics-Projects/Week of July 9 2023/Day 1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54E26E8E-7A54-8B4B-9E4F-B246F2684482}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8453C4B1-30A0-8E49-9ACF-BC92214D7791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" xr2:uid="{3E4B7A29-3A18-9B47-8AF0-A2A901AA8D72}"/>
+    <workbookView xWindow="1500" yWindow="820" windowWidth="46040" windowHeight="25740" xr2:uid="{3E4B7A29-3A18-9B47-8AF0-A2A901AA8D72}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -317,7 +317,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -405,6 +405,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -423,17 +438,10 @@
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="16" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -450,6 +458,13 @@
     <xf numFmtId="164" fontId="10" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="10" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -767,7 +782,7 @@
   <dimension ref="A1:Z48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="Q23" sqref="Q23"/>
+      <selection activeCell="P6" sqref="P6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -788,28 +803,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="A1" s="34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
     </row>
     <row r="2" spans="1:26" ht="21" x14ac:dyDescent="0.25">
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
       <c r="F2" s="10"/>
       <c r="G2" s="11"/>
       <c r="H2" s="9"/>
       <c r="I2" s="9"/>
-      <c r="J2" s="22" t="s">
+      <c r="J2" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
@@ -819,16 +834,16 @@
       <c r="C3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="G3" s="20" t="s">
+      <c r="G3" s="16" t="s">
         <v>47</v>
       </c>
       <c r="H3" s="8"/>
@@ -836,16 +851,16 @@
       <c r="J3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="K3" s="14" t="s">
+      <c r="K3" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="L3" s="16" t="s">
+      <c r="L3" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="M3" s="18" t="s">
+      <c r="M3" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="N3" s="20" t="s">
+      <c r="N3" s="16" t="s">
         <v>47</v>
       </c>
       <c r="O3" s="4"/>
@@ -866,39 +881,39 @@
         <v>2</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="13">
+      <c r="C4" s="35">
         <v>180</v>
       </c>
-      <c r="D4" s="15">
+      <c r="D4" s="36">
         <f>180-C4</f>
         <v>0</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="37">
         <v>5</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="38">
         <f t="shared" ref="F4:F42" si="0">(C4-D4)/180</f>
         <v>1</v>
       </c>
-      <c r="G4" s="21">
+      <c r="G4" s="39">
         <f t="shared" ref="G4:G42" si="1">E4/C4</f>
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="35">
         <v>177</v>
       </c>
-      <c r="K4" s="15">
+      <c r="K4" s="36">
         <f>180-J4</f>
         <v>3</v>
       </c>
-      <c r="L4" s="17">
-        <v>2</v>
-      </c>
-      <c r="M4" s="19">
+      <c r="L4" s="37">
+        <v>2</v>
+      </c>
+      <c r="M4" s="38">
         <f>(J4-K4)/180</f>
         <v>0.96666666666666667</v>
       </c>
-      <c r="N4" s="21">
+      <c r="N4" s="39">
         <f>L4/J4</f>
         <v>1.1299435028248588E-2</v>
       </c>
@@ -908,39 +923,39 @@
         <v>3</v>
       </c>
       <c r="B5" s="2"/>
-      <c r="C5" s="13">
+      <c r="C5" s="35">
         <v>153</v>
       </c>
-      <c r="D5" s="15">
+      <c r="D5" s="36">
         <f t="shared" ref="D5:D42" si="2">180-C5</f>
         <v>27</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="37">
         <v>3</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="38">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="G5" s="21">
+      <c r="G5" s="39">
         <f t="shared" si="1"/>
         <v>1.9607843137254902E-2</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="35">
         <v>179</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K5" s="36">
         <f t="shared" ref="K5:K42" si="3">180-J5</f>
         <v>1</v>
       </c>
-      <c r="L5" s="17">
+      <c r="L5" s="37">
         <v>4</v>
       </c>
-      <c r="M5" s="19">
+      <c r="M5" s="38">
         <f t="shared" ref="M5:M42" si="4">(J5-K5)/180</f>
         <v>0.98888888888888893</v>
       </c>
-      <c r="N5" s="21">
+      <c r="N5" s="39">
         <f t="shared" ref="N5:N42" si="5">L5/J5</f>
         <v>2.23463687150838E-2</v>
       </c>
@@ -950,39 +965,39 @@
         <v>4</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="13">
+      <c r="C6" s="35">
         <v>176</v>
       </c>
-      <c r="D6" s="15">
+      <c r="D6" s="36">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="E6" s="17">
+      <c r="E6" s="37">
         <v>3</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="38">
         <f t="shared" si="0"/>
         <v>0.9555555555555556</v>
       </c>
-      <c r="G6" s="21">
+      <c r="G6" s="39">
         <f t="shared" si="1"/>
         <v>1.7045454545454544E-2</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="35">
         <v>174</v>
       </c>
-      <c r="K6" s="15">
+      <c r="K6" s="36">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6" s="37">
         <v>4</v>
       </c>
-      <c r="M6" s="19">
+      <c r="M6" s="38">
         <f t="shared" si="4"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="N6" s="21">
+      <c r="N6" s="39">
         <f t="shared" si="5"/>
         <v>2.2988505747126436E-2</v>
       </c>
@@ -992,39 +1007,39 @@
         <v>5</v>
       </c>
       <c r="B7" s="2"/>
-      <c r="C7" s="13">
+      <c r="C7" s="35">
         <v>178</v>
       </c>
-      <c r="D7" s="15">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="E7" s="17">
-        <v>0</v>
-      </c>
-      <c r="F7" s="19">
+      <c r="D7" s="36">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E7" s="37">
+        <v>0</v>
+      </c>
+      <c r="F7" s="38">
         <f t="shared" si="0"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="G7" s="21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J7" s="13">
+      <c r="G7" s="39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="35">
         <v>180</v>
       </c>
-      <c r="K7" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L7" s="17">
-        <v>2</v>
-      </c>
-      <c r="M7" s="19">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="N7" s="21">
+      <c r="K7" s="36">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L7" s="37">
+        <v>2</v>
+      </c>
+      <c r="M7" s="38">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N7" s="39">
         <f t="shared" si="5"/>
         <v>1.1111111111111112E-2</v>
       </c>
@@ -1034,39 +1049,39 @@
         <v>6</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="13">
+      <c r="C8" s="35">
         <v>179</v>
       </c>
-      <c r="D8" s="15">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E8" s="17">
-        <v>2</v>
-      </c>
-      <c r="F8" s="19">
+      <c r="D8" s="36">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="37">
+        <v>2</v>
+      </c>
+      <c r="F8" s="38">
         <f t="shared" si="0"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="39">
         <f t="shared" si="1"/>
         <v>1.11731843575419E-2</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="35">
         <v>174</v>
       </c>
-      <c r="K8" s="15">
+      <c r="K8" s="36">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="37">
         <v>4</v>
       </c>
-      <c r="M8" s="19">
+      <c r="M8" s="38">
         <f t="shared" si="4"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="N8" s="21">
+      <c r="N8" s="39">
         <f t="shared" si="5"/>
         <v>2.2988505747126436E-2</v>
       </c>
@@ -1076,39 +1091,39 @@
         <v>7</v>
       </c>
       <c r="B9" s="2"/>
-      <c r="C9" s="13">
+      <c r="C9" s="35">
         <v>180</v>
       </c>
-      <c r="D9" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E9" s="17">
-        <v>1</v>
-      </c>
-      <c r="F9" s="19">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G9" s="21">
+      <c r="D9" s="36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="37">
+        <v>1</v>
+      </c>
+      <c r="F9" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G9" s="39">
         <f t="shared" si="1"/>
         <v>5.5555555555555558E-3</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="35">
         <v>178</v>
       </c>
-      <c r="K9" s="15">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L9" s="17">
-        <v>2</v>
-      </c>
-      <c r="M9" s="19">
+      <c r="K9" s="36">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L9" s="37">
+        <v>2</v>
+      </c>
+      <c r="M9" s="38">
         <f t="shared" si="4"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="N9" s="21">
+      <c r="N9" s="39">
         <f t="shared" si="5"/>
         <v>1.1235955056179775E-2</v>
       </c>
@@ -1118,39 +1133,39 @@
         <v>8</v>
       </c>
       <c r="B10" s="2"/>
-      <c r="C10" s="13">
+      <c r="C10" s="35">
         <v>168</v>
       </c>
-      <c r="D10" s="15">
+      <c r="D10" s="36">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="E10" s="17">
-        <v>2</v>
-      </c>
-      <c r="F10" s="19">
+      <c r="E10" s="37">
+        <v>2</v>
+      </c>
+      <c r="F10" s="38">
         <f t="shared" si="0"/>
         <v>0.8666666666666667</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="39">
         <f t="shared" si="1"/>
         <v>1.1904761904761904E-2</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="35">
         <v>179</v>
       </c>
-      <c r="K10" s="15">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L10" s="17">
-        <v>1</v>
-      </c>
-      <c r="M10" s="19">
+      <c r="K10" s="36">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L10" s="37">
+        <v>1</v>
+      </c>
+      <c r="M10" s="38">
         <f t="shared" si="4"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="N10" s="21">
+      <c r="N10" s="39">
         <f t="shared" si="5"/>
         <v>5.5865921787709499E-3</v>
       </c>
@@ -1160,39 +1175,39 @@
         <v>9</v>
       </c>
       <c r="B11" s="2"/>
-      <c r="C11" s="13">
+      <c r="C11" s="35">
         <v>178</v>
       </c>
-      <c r="D11" s="15">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="E11" s="17">
+      <c r="D11" s="36">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E11" s="37">
         <v>15</v>
       </c>
-      <c r="F11" s="19">
+      <c r="F11" s="38">
         <f t="shared" si="0"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="G11" s="21">
+      <c r="G11" s="39">
         <f t="shared" si="1"/>
         <v>8.4269662921348312E-2</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="35">
         <v>177</v>
       </c>
-      <c r="K11" s="15">
+      <c r="K11" s="36">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="L11" s="17">
-        <v>0</v>
-      </c>
-      <c r="M11" s="19">
+      <c r="L11" s="37">
+        <v>0</v>
+      </c>
+      <c r="M11" s="38">
         <f t="shared" si="4"/>
         <v>0.96666666666666667</v>
       </c>
-      <c r="N11" s="21">
+      <c r="N11" s="39">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1202,39 +1217,39 @@
         <v>10</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="13">
+      <c r="C12" s="35">
         <v>174</v>
       </c>
-      <c r="D12" s="15">
+      <c r="D12" s="36">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="E12" s="17">
-        <v>2</v>
-      </c>
-      <c r="F12" s="19">
+      <c r="E12" s="37">
+        <v>2</v>
+      </c>
+      <c r="F12" s="38">
         <f t="shared" si="0"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="G12" s="21">
+      <c r="G12" s="39">
         <f t="shared" si="1"/>
         <v>1.1494252873563218E-2</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="35">
         <v>180</v>
       </c>
-      <c r="K12" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L12" s="17">
+      <c r="K12" s="36">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="37">
         <v>6</v>
       </c>
-      <c r="M12" s="19">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="N12" s="21">
+      <c r="M12" s="38">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N12" s="39">
         <f t="shared" si="5"/>
         <v>3.3333333333333333E-2</v>
       </c>
@@ -1244,39 +1259,39 @@
         <v>11</v>
       </c>
       <c r="B13" s="2"/>
-      <c r="C13" s="13">
+      <c r="C13" s="35">
         <v>180</v>
       </c>
-      <c r="D13" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E13" s="17">
-        <v>1</v>
-      </c>
-      <c r="F13" s="19">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G13" s="21">
+      <c r="D13" s="36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E13" s="37">
+        <v>1</v>
+      </c>
+      <c r="F13" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G13" s="39">
         <f t="shared" si="1"/>
         <v>5.5555555555555558E-3</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13" s="35">
         <v>176</v>
       </c>
-      <c r="K13" s="15">
+      <c r="K13" s="36">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="L13" s="17">
+      <c r="L13" s="37">
         <v>3</v>
       </c>
-      <c r="M13" s="19">
+      <c r="M13" s="38">
         <f t="shared" si="4"/>
         <v>0.9555555555555556</v>
       </c>
-      <c r="N13" s="21">
+      <c r="N13" s="39">
         <f t="shared" si="5"/>
         <v>1.7045454545454544E-2</v>
       </c>
@@ -1286,39 +1301,39 @@
         <v>12</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="13">
+      <c r="C14" s="35">
         <v>174</v>
       </c>
-      <c r="D14" s="15">
+      <c r="D14" s="36">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="E14" s="17">
-        <v>0</v>
-      </c>
-      <c r="F14" s="19">
+      <c r="E14" s="37">
+        <v>0</v>
+      </c>
+      <c r="F14" s="38">
         <f t="shared" si="0"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="G14" s="21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J14" s="13">
+      <c r="G14" s="39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J14" s="35">
         <v>174</v>
       </c>
-      <c r="K14" s="15">
+      <c r="K14" s="36">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="L14" s="17">
+      <c r="L14" s="37">
         <v>5</v>
       </c>
-      <c r="M14" s="19">
+      <c r="M14" s="38">
         <f t="shared" si="4"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="N14" s="21">
+      <c r="N14" s="39">
         <f t="shared" si="5"/>
         <v>2.8735632183908046E-2</v>
       </c>
@@ -1328,39 +1343,39 @@
         <v>13</v>
       </c>
       <c r="B15" s="2"/>
-      <c r="C15" s="13">
+      <c r="C15" s="35">
         <v>179</v>
       </c>
-      <c r="D15" s="15">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E15" s="17">
-        <v>2</v>
-      </c>
-      <c r="F15" s="19">
+      <c r="D15" s="36">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E15" s="37">
+        <v>2</v>
+      </c>
+      <c r="F15" s="38">
         <f t="shared" si="0"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="G15" s="21">
+      <c r="G15" s="39">
         <f t="shared" si="1"/>
         <v>1.11731843575419E-2</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="35">
         <v>178</v>
       </c>
-      <c r="K15" s="15">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L15" s="17">
+      <c r="K15" s="36">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L15" s="37">
         <v>3</v>
       </c>
-      <c r="M15" s="19">
+      <c r="M15" s="38">
         <f t="shared" si="4"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="N15" s="21">
+      <c r="N15" s="39">
         <f t="shared" si="5"/>
         <v>1.6853932584269662E-2</v>
       </c>
@@ -1370,39 +1385,39 @@
         <v>14</v>
       </c>
       <c r="B16" s="2"/>
-      <c r="C16" s="13">
+      <c r="C16" s="35">
         <v>176</v>
       </c>
-      <c r="D16" s="15">
+      <c r="D16" s="36">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="E16" s="17">
+      <c r="E16" s="37">
         <v>5</v>
       </c>
-      <c r="F16" s="19">
+      <c r="F16" s="38">
         <f t="shared" si="0"/>
         <v>0.9555555555555556</v>
       </c>
-      <c r="G16" s="21">
+      <c r="G16" s="39">
         <f t="shared" si="1"/>
         <v>2.8409090909090908E-2</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="35">
         <v>179</v>
       </c>
-      <c r="K16" s="15">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L16" s="17">
-        <v>2</v>
-      </c>
-      <c r="M16" s="19">
+      <c r="K16" s="36">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L16" s="37">
+        <v>2</v>
+      </c>
+      <c r="M16" s="38">
         <f t="shared" si="4"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="N16" s="21">
+      <c r="N16" s="39">
         <f t="shared" si="5"/>
         <v>1.11731843575419E-2</v>
       </c>
@@ -1412,39 +1427,39 @@
         <v>15</v>
       </c>
       <c r="B17" s="2"/>
-      <c r="C17" s="13">
+      <c r="C17" s="35">
         <v>178</v>
       </c>
-      <c r="D17" s="15">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="E17" s="17">
-        <v>0</v>
-      </c>
-      <c r="F17" s="19">
+      <c r="D17" s="36">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E17" s="37">
+        <v>0</v>
+      </c>
+      <c r="F17" s="38">
         <f t="shared" si="0"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="G17" s="21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J17" s="13">
+      <c r="G17" s="39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="35">
         <v>178</v>
       </c>
-      <c r="K17" s="15">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L17" s="17">
-        <v>0</v>
-      </c>
-      <c r="M17" s="19">
+      <c r="K17" s="36">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L17" s="37">
+        <v>0</v>
+      </c>
+      <c r="M17" s="38">
         <f t="shared" si="4"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="N17" s="21">
+      <c r="N17" s="39">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1454,39 +1469,39 @@
         <v>16</v>
       </c>
       <c r="B18" s="2"/>
-      <c r="C18" s="13">
+      <c r="C18" s="35">
         <v>177</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D18" s="36">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="E18" s="17">
+      <c r="E18" s="37">
         <v>4</v>
       </c>
-      <c r="F18" s="19">
+      <c r="F18" s="38">
         <f t="shared" si="0"/>
         <v>0.96666666666666667</v>
       </c>
-      <c r="G18" s="21">
+      <c r="G18" s="39">
         <f t="shared" si="1"/>
         <v>2.2598870056497175E-2</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="35">
         <v>174</v>
       </c>
-      <c r="K18" s="15">
+      <c r="K18" s="36">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="L18" s="17">
+      <c r="L18" s="37">
         <v>5</v>
       </c>
-      <c r="M18" s="19">
+      <c r="M18" s="38">
         <f t="shared" si="4"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="N18" s="21">
+      <c r="N18" s="39">
         <f t="shared" si="5"/>
         <v>2.8735632183908046E-2</v>
       </c>
@@ -1496,39 +1511,39 @@
         <v>17</v>
       </c>
       <c r="B19" s="2"/>
-      <c r="C19" s="13">
+      <c r="C19" s="35">
         <v>180</v>
       </c>
-      <c r="D19" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E19" s="17">
-        <v>2</v>
-      </c>
-      <c r="F19" s="19">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G19" s="21">
+      <c r="D19" s="36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E19" s="37">
+        <v>2</v>
+      </c>
+      <c r="F19" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G19" s="39">
         <f t="shared" si="1"/>
         <v>1.1111111111111112E-2</v>
       </c>
-      <c r="J19" s="13">
+      <c r="J19" s="35">
         <v>177</v>
       </c>
-      <c r="K19" s="15">
+      <c r="K19" s="36">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="L19" s="17">
+      <c r="L19" s="37">
         <v>6</v>
       </c>
-      <c r="M19" s="19">
+      <c r="M19" s="38">
         <f t="shared" si="4"/>
         <v>0.96666666666666667</v>
       </c>
-      <c r="N19" s="21">
+      <c r="N19" s="39">
         <f t="shared" si="5"/>
         <v>3.3898305084745763E-2</v>
       </c>
@@ -1538,39 +1553,39 @@
         <v>18</v>
       </c>
       <c r="B20" s="2"/>
-      <c r="C20" s="13">
+      <c r="C20" s="35">
         <v>172</v>
       </c>
-      <c r="D20" s="15">
+      <c r="D20" s="36">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="E20" s="17">
-        <v>0</v>
-      </c>
-      <c r="F20" s="19">
+      <c r="E20" s="37">
+        <v>0</v>
+      </c>
+      <c r="F20" s="38">
         <f t="shared" si="0"/>
         <v>0.91111111111111109</v>
       </c>
-      <c r="G20" s="21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J20" s="13">
+      <c r="G20" s="39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="35">
         <v>178</v>
       </c>
-      <c r="K20" s="15">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L20" s="17">
-        <v>2</v>
-      </c>
-      <c r="M20" s="19">
+      <c r="K20" s="36">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L20" s="37">
+        <v>2</v>
+      </c>
+      <c r="M20" s="38">
         <f t="shared" si="4"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="N20" s="21">
+      <c r="N20" s="39">
         <f t="shared" si="5"/>
         <v>1.1235955056179775E-2</v>
       </c>
@@ -1580,39 +1595,39 @@
         <v>19</v>
       </c>
       <c r="B21" s="2"/>
-      <c r="C21" s="13">
+      <c r="C21" s="35">
         <v>178</v>
       </c>
-      <c r="D21" s="15">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="E21" s="17">
+      <c r="D21" s="36">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E21" s="37">
         <v>5</v>
       </c>
-      <c r="F21" s="19">
+      <c r="F21" s="38">
         <f t="shared" si="0"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="G21" s="21">
+      <c r="G21" s="39">
         <f t="shared" si="1"/>
         <v>2.8089887640449437E-2</v>
       </c>
-      <c r="J21" s="13">
+      <c r="J21" s="35">
         <v>169</v>
       </c>
-      <c r="K21" s="15">
+      <c r="K21" s="36">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="L21" s="17">
+      <c r="L21" s="37">
         <v>3</v>
       </c>
-      <c r="M21" s="19">
+      <c r="M21" s="38">
         <f t="shared" si="4"/>
         <v>0.87777777777777777</v>
       </c>
-      <c r="N21" s="21">
+      <c r="N21" s="39">
         <f t="shared" si="5"/>
         <v>1.7751479289940829E-2</v>
       </c>
@@ -1622,39 +1637,39 @@
         <v>20</v>
       </c>
       <c r="B22" s="2"/>
-      <c r="C22" s="13">
+      <c r="C22" s="35">
         <v>172</v>
       </c>
-      <c r="D22" s="15">
+      <c r="D22" s="36">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="E22" s="17">
-        <v>2</v>
-      </c>
-      <c r="F22" s="19">
+      <c r="E22" s="37">
+        <v>2</v>
+      </c>
+      <c r="F22" s="38">
         <f t="shared" si="0"/>
         <v>0.91111111111111109</v>
       </c>
-      <c r="G22" s="21">
+      <c r="G22" s="39">
         <f t="shared" si="1"/>
         <v>1.1627906976744186E-2</v>
       </c>
-      <c r="J22" s="13">
+      <c r="J22" s="35">
         <v>177</v>
       </c>
-      <c r="K22" s="15">
+      <c r="K22" s="36">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="L22" s="17">
+      <c r="L22" s="37">
         <v>16</v>
       </c>
-      <c r="M22" s="19">
+      <c r="M22" s="38">
         <f t="shared" si="4"/>
         <v>0.96666666666666667</v>
       </c>
-      <c r="N22" s="21">
+      <c r="N22" s="39">
         <f t="shared" si="5"/>
         <v>9.03954802259887E-2</v>
       </c>
@@ -1664,39 +1679,39 @@
         <v>21</v>
       </c>
       <c r="B23" s="2"/>
-      <c r="C23" s="13">
+      <c r="C23" s="35">
         <v>178</v>
       </c>
-      <c r="D23" s="15">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="E23" s="17">
-        <v>2</v>
-      </c>
-      <c r="F23" s="19">
+      <c r="D23" s="36">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E23" s="37">
+        <v>2</v>
+      </c>
+      <c r="F23" s="38">
         <f t="shared" si="0"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="G23" s="21">
+      <c r="G23" s="39">
         <f t="shared" si="1"/>
         <v>1.1235955056179775E-2</v>
       </c>
-      <c r="J23" s="13">
+      <c r="J23" s="35">
         <v>179</v>
       </c>
-      <c r="K23" s="15">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L23" s="17">
-        <v>2</v>
-      </c>
-      <c r="M23" s="19">
+      <c r="K23" s="36">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L23" s="37">
+        <v>2</v>
+      </c>
+      <c r="M23" s="38">
         <f t="shared" si="4"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="N23" s="21">
+      <c r="N23" s="39">
         <f t="shared" si="5"/>
         <v>1.11731843575419E-2</v>
       </c>
@@ -1706,39 +1721,39 @@
         <v>22</v>
       </c>
       <c r="B24" s="2"/>
-      <c r="C24" s="13">
+      <c r="C24" s="35">
         <v>174</v>
       </c>
-      <c r="D24" s="15">
+      <c r="D24" s="36">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="E24" s="17">
-        <v>0</v>
-      </c>
-      <c r="F24" s="19">
+      <c r="E24" s="37">
+        <v>0</v>
+      </c>
+      <c r="F24" s="38">
         <f t="shared" si="0"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="G24" s="21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J24" s="13">
+      <c r="G24" s="39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="35">
         <v>180</v>
       </c>
-      <c r="K24" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L24" s="17">
+      <c r="K24" s="36">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L24" s="37">
         <v>5</v>
       </c>
-      <c r="M24" s="19">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="N24" s="21">
+      <c r="M24" s="38">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N24" s="39">
         <f t="shared" si="5"/>
         <v>2.7777777777777776E-2</v>
       </c>
@@ -1748,39 +1763,39 @@
         <v>23</v>
       </c>
       <c r="B25" s="2"/>
-      <c r="C25" s="13">
+      <c r="C25" s="35">
         <v>179</v>
       </c>
-      <c r="D25" s="15">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E25" s="17">
+      <c r="D25" s="36">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E25" s="37">
         <v>6</v>
       </c>
-      <c r="F25" s="19">
+      <c r="F25" s="38">
         <f t="shared" si="0"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="G25" s="21">
+      <c r="G25" s="39">
         <f t="shared" si="1"/>
         <v>3.3519553072625698E-2</v>
       </c>
-      <c r="J25" s="13">
+      <c r="J25" s="35">
         <v>176</v>
       </c>
-      <c r="K25" s="15">
+      <c r="K25" s="36">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="L25" s="17">
-        <v>0</v>
-      </c>
-      <c r="M25" s="19">
+      <c r="L25" s="37">
+        <v>0</v>
+      </c>
+      <c r="M25" s="38">
         <f t="shared" si="4"/>
         <v>0.9555555555555556</v>
       </c>
-      <c r="N25" s="21">
+      <c r="N25" s="39">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -1790,39 +1805,39 @@
         <v>24</v>
       </c>
       <c r="B26" s="2"/>
-      <c r="C26" s="13">
+      <c r="C26" s="35">
         <v>174</v>
       </c>
-      <c r="D26" s="15">
+      <c r="D26" s="36">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="E26" s="17">
+      <c r="E26" s="37">
         <v>13</v>
       </c>
-      <c r="F26" s="19">
+      <c r="F26" s="38">
         <f t="shared" si="0"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="G26" s="21">
+      <c r="G26" s="39">
         <f t="shared" si="1"/>
         <v>7.4712643678160925E-2</v>
       </c>
-      <c r="J26" s="13">
+      <c r="J26" s="35">
         <v>172</v>
       </c>
-      <c r="K26" s="15">
+      <c r="K26" s="36">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="L26" s="17">
-        <v>2</v>
-      </c>
-      <c r="M26" s="19">
+      <c r="L26" s="37">
+        <v>2</v>
+      </c>
+      <c r="M26" s="38">
         <f t="shared" si="4"/>
         <v>0.91111111111111109</v>
       </c>
-      <c r="N26" s="21">
+      <c r="N26" s="39">
         <f t="shared" si="5"/>
         <v>1.1627906976744186E-2</v>
       </c>
@@ -1832,39 +1847,39 @@
         <v>35</v>
       </c>
       <c r="B27" s="2"/>
-      <c r="C27" s="13">
+      <c r="C27" s="35">
         <v>180</v>
       </c>
-      <c r="D27" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E27" s="17">
-        <v>2</v>
-      </c>
-      <c r="F27" s="19">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G27" s="21">
+      <c r="D27" s="36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E27" s="37">
+        <v>2</v>
+      </c>
+      <c r="F27" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G27" s="39">
         <f t="shared" si="1"/>
         <v>1.1111111111111112E-2</v>
       </c>
-      <c r="J27" s="13">
+      <c r="J27" s="35">
         <v>179</v>
       </c>
-      <c r="K27" s="15">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L27" s="17">
+      <c r="K27" s="36">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L27" s="37">
         <v>6</v>
       </c>
-      <c r="M27" s="19">
+      <c r="M27" s="38">
         <f t="shared" si="4"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="N27" s="21">
+      <c r="N27" s="39">
         <f t="shared" si="5"/>
         <v>3.3519553072625698E-2</v>
       </c>
@@ -1874,39 +1889,39 @@
         <v>25</v>
       </c>
       <c r="B28" s="2"/>
-      <c r="C28" s="13">
+      <c r="C28" s="35">
         <v>177</v>
       </c>
-      <c r="D28" s="15">
+      <c r="D28" s="36">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="E28" s="17">
+      <c r="E28" s="37">
         <v>4</v>
       </c>
-      <c r="F28" s="19">
+      <c r="F28" s="38">
         <f t="shared" si="0"/>
         <v>0.96666666666666667</v>
       </c>
-      <c r="G28" s="21">
+      <c r="G28" s="39">
         <f t="shared" si="1"/>
         <v>2.2598870056497175E-2</v>
       </c>
-      <c r="J28" s="13">
+      <c r="J28" s="35">
         <v>178</v>
       </c>
-      <c r="K28" s="15">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L28" s="17">
+      <c r="K28" s="36">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L28" s="37">
         <v>4</v>
       </c>
-      <c r="M28" s="19">
+      <c r="M28" s="38">
         <f t="shared" si="4"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="N28" s="21">
+      <c r="N28" s="39">
         <f t="shared" si="5"/>
         <v>2.247191011235955E-2</v>
       </c>
@@ -1916,39 +1931,39 @@
         <v>26</v>
       </c>
       <c r="B29" s="2"/>
-      <c r="C29" s="13">
+      <c r="C29" s="35">
         <v>176</v>
       </c>
-      <c r="D29" s="15">
+      <c r="D29" s="36">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="E29" s="17">
-        <v>0</v>
-      </c>
-      <c r="F29" s="19">
+      <c r="E29" s="37">
+        <v>0</v>
+      </c>
+      <c r="F29" s="38">
         <f t="shared" si="0"/>
         <v>0.9555555555555556</v>
       </c>
-      <c r="G29" s="21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J29" s="13">
+      <c r="G29" s="39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J29" s="35">
         <v>177</v>
       </c>
-      <c r="K29" s="15">
+      <c r="K29" s="36">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="L29" s="17">
-        <v>2</v>
-      </c>
-      <c r="M29" s="19">
+      <c r="L29" s="37">
+        <v>2</v>
+      </c>
+      <c r="M29" s="38">
         <f t="shared" si="4"/>
         <v>0.96666666666666667</v>
       </c>
-      <c r="N29" s="21">
+      <c r="N29" s="39">
         <f t="shared" si="5"/>
         <v>1.1299435028248588E-2</v>
       </c>
@@ -1958,39 +1973,39 @@
         <v>27</v>
       </c>
       <c r="B30" s="2"/>
-      <c r="C30" s="13">
+      <c r="C30" s="35">
         <v>180</v>
       </c>
-      <c r="D30" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E30" s="17">
+      <c r="D30" s="36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E30" s="37">
         <v>5</v>
       </c>
-      <c r="F30" s="19">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G30" s="21">
+      <c r="F30" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G30" s="39">
         <f t="shared" si="1"/>
         <v>2.7777777777777776E-2</v>
       </c>
-      <c r="J30" s="13">
+      <c r="J30" s="35">
         <v>180</v>
       </c>
-      <c r="K30" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L30" s="17">
+      <c r="K30" s="36">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="37">
         <v>6</v>
       </c>
-      <c r="M30" s="19">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="N30" s="21">
+      <c r="M30" s="38">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N30" s="39">
         <f t="shared" si="5"/>
         <v>3.3333333333333333E-2</v>
       </c>
@@ -2000,39 +2015,39 @@
         <v>28</v>
       </c>
       <c r="B31" s="2"/>
-      <c r="C31" s="13">
+      <c r="C31" s="35">
         <v>174</v>
       </c>
-      <c r="D31" s="15">
+      <c r="D31" s="36">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="E31" s="17">
+      <c r="E31" s="37">
         <v>5</v>
       </c>
-      <c r="F31" s="19">
+      <c r="F31" s="38">
         <f t="shared" si="0"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="G31" s="21">
+      <c r="G31" s="39">
         <f t="shared" si="1"/>
         <v>2.8735632183908046E-2</v>
       </c>
-      <c r="J31" s="13">
+      <c r="J31" s="35">
         <v>177</v>
       </c>
-      <c r="K31" s="15">
+      <c r="K31" s="36">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="L31" s="17">
-        <v>2</v>
-      </c>
-      <c r="M31" s="19">
+      <c r="L31" s="37">
+        <v>2</v>
+      </c>
+      <c r="M31" s="38">
         <f t="shared" si="4"/>
         <v>0.96666666666666667</v>
       </c>
-      <c r="N31" s="21">
+      <c r="N31" s="39">
         <f t="shared" si="5"/>
         <v>1.1299435028248588E-2</v>
       </c>
@@ -2042,39 +2057,39 @@
         <v>29</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="13">
+      <c r="C32" s="35">
         <v>177</v>
       </c>
-      <c r="D32" s="15">
+      <c r="D32" s="36">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="E32" s="17">
-        <v>2</v>
-      </c>
-      <c r="F32" s="19">
+      <c r="E32" s="37">
+        <v>2</v>
+      </c>
+      <c r="F32" s="38">
         <f t="shared" si="0"/>
         <v>0.96666666666666667</v>
       </c>
-      <c r="G32" s="21">
+      <c r="G32" s="39">
         <f t="shared" si="1"/>
         <v>1.1299435028248588E-2</v>
       </c>
-      <c r="J32" s="13">
+      <c r="J32" s="35">
         <v>172</v>
       </c>
-      <c r="K32" s="15">
+      <c r="K32" s="36">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="L32" s="17">
+      <c r="L32" s="37">
         <v>4</v>
       </c>
-      <c r="M32" s="19">
+      <c r="M32" s="38">
         <f t="shared" si="4"/>
         <v>0.91111111111111109</v>
       </c>
-      <c r="N32" s="21">
+      <c r="N32" s="39">
         <f t="shared" si="5"/>
         <v>2.3255813953488372E-2</v>
       </c>
@@ -2084,39 +2099,39 @@
         <v>36</v>
       </c>
       <c r="B33" s="2"/>
-      <c r="C33" s="13">
+      <c r="C33" s="35">
         <v>180</v>
       </c>
-      <c r="D33" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E33" s="17">
-        <v>0</v>
-      </c>
-      <c r="F33" s="19">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G33" s="21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J33" s="13">
+      <c r="D33" s="36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E33" s="37">
+        <v>0</v>
+      </c>
+      <c r="F33" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G33" s="39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="35">
         <v>178</v>
       </c>
-      <c r="K33" s="15">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L33" s="17">
+      <c r="K33" s="36">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L33" s="37">
         <v>4</v>
       </c>
-      <c r="M33" s="19">
+      <c r="M33" s="38">
         <f t="shared" si="4"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="N33" s="21">
+      <c r="N33" s="39">
         <f t="shared" si="5"/>
         <v>2.247191011235955E-2</v>
       </c>
@@ -2126,39 +2141,39 @@
         <v>37</v>
       </c>
       <c r="B34" s="2"/>
-      <c r="C34" s="13">
+      <c r="C34" s="35">
         <v>174</v>
       </c>
-      <c r="D34" s="15">
+      <c r="D34" s="36">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="E34" s="17">
-        <v>2</v>
-      </c>
-      <c r="F34" s="19">
+      <c r="E34" s="37">
+        <v>2</v>
+      </c>
+      <c r="F34" s="38">
         <f t="shared" si="0"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="G34" s="21">
+      <c r="G34" s="39">
         <f t="shared" si="1"/>
         <v>1.1494252873563218E-2</v>
       </c>
-      <c r="J34" s="13">
+      <c r="J34" s="35">
         <v>178</v>
       </c>
-      <c r="K34" s="15">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="L34" s="17">
-        <v>1</v>
-      </c>
-      <c r="M34" s="19">
+      <c r="K34" s="36">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L34" s="37">
+        <v>1</v>
+      </c>
+      <c r="M34" s="38">
         <f t="shared" si="4"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="N34" s="21">
+      <c r="N34" s="39">
         <f t="shared" si="5"/>
         <v>5.6179775280898875E-3</v>
       </c>
@@ -2168,39 +2183,39 @@
         <v>38</v>
       </c>
       <c r="B35" s="2"/>
-      <c r="C35" s="13">
+      <c r="C35" s="35">
         <v>179</v>
       </c>
-      <c r="D35" s="15">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E35" s="17">
-        <v>1</v>
-      </c>
-      <c r="F35" s="19">
+      <c r="D35" s="36">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E35" s="37">
+        <v>1</v>
+      </c>
+      <c r="F35" s="38">
         <f t="shared" si="0"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="G35" s="21">
+      <c r="G35" s="39">
         <f t="shared" si="1"/>
         <v>5.5865921787709499E-3</v>
       </c>
-      <c r="J35" s="13">
+      <c r="J35" s="35">
         <v>179</v>
       </c>
-      <c r="K35" s="15">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L35" s="17">
-        <v>0</v>
-      </c>
-      <c r="M35" s="19">
+      <c r="K35" s="36">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L35" s="37">
+        <v>0</v>
+      </c>
+      <c r="M35" s="38">
         <f t="shared" si="4"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="N35" s="21">
+      <c r="N35" s="39">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2210,39 +2225,39 @@
         <v>30</v>
       </c>
       <c r="B36" s="2"/>
-      <c r="C36" s="13">
+      <c r="C36" s="35">
         <v>180</v>
       </c>
-      <c r="D36" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E36" s="17">
+      <c r="D36" s="36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E36" s="37">
         <v>3</v>
       </c>
-      <c r="F36" s="19">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G36" s="21">
+      <c r="F36" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G36" s="39">
         <f t="shared" si="1"/>
         <v>1.6666666666666666E-2</v>
       </c>
-      <c r="J36" s="13">
+      <c r="J36" s="35">
         <v>179</v>
       </c>
-      <c r="K36" s="15">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L36" s="17">
-        <v>2</v>
-      </c>
-      <c r="M36" s="19">
+      <c r="K36" s="36">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L36" s="37">
+        <v>2</v>
+      </c>
+      <c r="M36" s="38">
         <f t="shared" si="4"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="N36" s="21">
+      <c r="N36" s="39">
         <f t="shared" si="5"/>
         <v>1.11731843575419E-2</v>
       </c>
@@ -2252,39 +2267,39 @@
         <v>31</v>
       </c>
       <c r="B37" s="2"/>
-      <c r="C37" s="13">
+      <c r="C37" s="35">
         <v>174</v>
       </c>
-      <c r="D37" s="15">
+      <c r="D37" s="36">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="E37" s="17">
-        <v>0</v>
-      </c>
-      <c r="F37" s="19">
+      <c r="E37" s="37">
+        <v>0</v>
+      </c>
+      <c r="F37" s="38">
         <f t="shared" si="0"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="G37" s="21">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="J37" s="13">
+      <c r="G37" s="39">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="35">
         <v>180</v>
       </c>
-      <c r="K37" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L37" s="17">
+      <c r="K37" s="36">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L37" s="37">
         <v>4</v>
       </c>
-      <c r="M37" s="19">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="N37" s="21">
+      <c r="M37" s="38">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N37" s="39">
         <f t="shared" si="5"/>
         <v>2.2222222222222223E-2</v>
       </c>
@@ -2294,39 +2309,39 @@
         <v>32</v>
       </c>
       <c r="B38" s="2"/>
-      <c r="C38" s="13">
+      <c r="C38" s="35">
         <v>178</v>
       </c>
-      <c r="D38" s="15">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="E38" s="17">
-        <v>2</v>
-      </c>
-      <c r="F38" s="19">
+      <c r="D38" s="36">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E38" s="37">
+        <v>2</v>
+      </c>
+      <c r="F38" s="38">
         <f t="shared" si="0"/>
         <v>0.97777777777777775</v>
       </c>
-      <c r="G38" s="21">
+      <c r="G38" s="39">
         <f t="shared" si="1"/>
         <v>1.1235955056179775E-2</v>
       </c>
-      <c r="J38" s="13">
+      <c r="J38" s="35">
         <v>174</v>
       </c>
-      <c r="K38" s="15">
+      <c r="K38" s="36">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="L38" s="17">
-        <v>0</v>
-      </c>
-      <c r="M38" s="19">
+      <c r="L38" s="37">
+        <v>0</v>
+      </c>
+      <c r="M38" s="38">
         <f t="shared" si="4"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="N38" s="21">
+      <c r="N38" s="39">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
@@ -2336,39 +2351,39 @@
         <v>33</v>
       </c>
       <c r="B39" s="2"/>
-      <c r="C39" s="13">
+      <c r="C39" s="35">
         <v>172</v>
       </c>
-      <c r="D39" s="15">
+      <c r="D39" s="36">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="E39" s="17">
+      <c r="E39" s="37">
         <v>4</v>
       </c>
-      <c r="F39" s="19">
+      <c r="F39" s="38">
         <f t="shared" si="0"/>
         <v>0.91111111111111109</v>
       </c>
-      <c r="G39" s="21">
+      <c r="G39" s="39">
         <f t="shared" si="1"/>
         <v>2.3255813953488372E-2</v>
       </c>
-      <c r="J39" s="13">
+      <c r="J39" s="35">
         <v>177</v>
       </c>
-      <c r="K39" s="15">
+      <c r="K39" s="36">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="L39" s="17">
+      <c r="L39" s="37">
         <v>6</v>
       </c>
-      <c r="M39" s="19">
+      <c r="M39" s="38">
         <f t="shared" si="4"/>
         <v>0.96666666666666667</v>
       </c>
-      <c r="N39" s="21">
+      <c r="N39" s="39">
         <f t="shared" si="5"/>
         <v>3.3898305084745763E-2</v>
       </c>
@@ -2378,39 +2393,39 @@
         <v>34</v>
       </c>
       <c r="B40" s="2"/>
-      <c r="C40" s="13">
+      <c r="C40" s="35">
         <v>179</v>
       </c>
-      <c r="D40" s="15">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="E40" s="17">
-        <v>1</v>
-      </c>
-      <c r="F40" s="19">
+      <c r="D40" s="36">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E40" s="37">
+        <v>1</v>
+      </c>
+      <c r="F40" s="38">
         <f t="shared" si="0"/>
         <v>0.98888888888888893</v>
       </c>
-      <c r="G40" s="21">
+      <c r="G40" s="39">
         <f t="shared" si="1"/>
         <v>5.5865921787709499E-3</v>
       </c>
-      <c r="J40" s="13">
+      <c r="J40" s="35">
         <v>180</v>
       </c>
-      <c r="K40" s="15">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L40" s="17">
-        <v>2</v>
-      </c>
-      <c r="M40" s="19">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="N40" s="21">
+      <c r="K40" s="36">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L40" s="37">
+        <v>2</v>
+      </c>
+      <c r="M40" s="38">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="N40" s="39">
         <f t="shared" si="5"/>
         <v>1.1111111111111112E-2</v>
       </c>
@@ -2420,39 +2435,39 @@
         <v>39</v>
       </c>
       <c r="B41" s="2"/>
-      <c r="C41" s="13">
+      <c r="C41" s="35">
         <v>180</v>
       </c>
-      <c r="D41" s="15">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="E41" s="17">
-        <v>2</v>
-      </c>
-      <c r="F41" s="19">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="G41" s="21">
+      <c r="D41" s="36">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E41" s="37">
+        <v>2</v>
+      </c>
+      <c r="F41" s="38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="G41" s="39">
         <f t="shared" si="1"/>
         <v>1.1111111111111112E-2</v>
       </c>
-      <c r="J41" s="13">
+      <c r="J41" s="35">
         <v>174</v>
       </c>
-      <c r="K41" s="15">
+      <c r="K41" s="36">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="L41" s="17">
+      <c r="L41" s="37">
         <v>5</v>
       </c>
-      <c r="M41" s="19">
+      <c r="M41" s="38">
         <f t="shared" si="4"/>
         <v>0.93333333333333335</v>
       </c>
-      <c r="N41" s="21">
+      <c r="N41" s="39">
         <f t="shared" si="5"/>
         <v>2.8735632183908046E-2</v>
       </c>
@@ -2462,39 +2477,39 @@
         <v>40</v>
       </c>
       <c r="B42" s="2"/>
-      <c r="C42" s="13">
+      <c r="C42" s="35">
         <v>177</v>
       </c>
-      <c r="D42" s="15">
+      <c r="D42" s="36">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="E42" s="17">
+      <c r="E42" s="37">
         <v>5</v>
       </c>
-      <c r="F42" s="19">
+      <c r="F42" s="38">
         <f t="shared" si="0"/>
         <v>0.96666666666666667</v>
       </c>
-      <c r="G42" s="21">
+      <c r="G42" s="39">
         <f t="shared" si="1"/>
         <v>2.8248587570621469E-2</v>
       </c>
-      <c r="J42" s="13">
+      <c r="J42" s="35">
         <v>170</v>
       </c>
-      <c r="K42" s="15">
+      <c r="K42" s="36">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="L42" s="17">
-        <v>1</v>
-      </c>
-      <c r="M42" s="19">
+      <c r="L42" s="37">
+        <v>1</v>
+      </c>
+      <c r="M42" s="38">
         <f t="shared" si="4"/>
         <v>0.88888888888888884</v>
       </c>
-      <c r="N42" s="21">
+      <c r="N42" s="39">
         <f t="shared" si="5"/>
         <v>5.8823529411764705E-3</v>
       </c>
@@ -2506,145 +2521,145 @@
       <c r="M43" s="6"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A44" s="24" t="s">
+      <c r="A44" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="25"/>
-      <c r="C44" s="26">
+      <c r="B44" s="18"/>
+      <c r="C44" s="19">
         <f>MAX(C4:C42)</f>
         <v>180</v>
       </c>
-      <c r="D44" s="26">
+      <c r="D44" s="19">
         <f>MAX(D4:D42)</f>
         <v>27</v>
       </c>
-      <c r="E44" s="26">
+      <c r="E44" s="19">
         <f>MAX(E4:E42)</f>
         <v>15</v>
       </c>
-      <c r="F44" s="27">
+      <c r="F44" s="20">
         <f>MAX(F4:F42)</f>
         <v>1</v>
       </c>
-      <c r="G44" s="27">
+      <c r="G44" s="20">
         <f>MAX(G4:G42)</f>
         <v>8.4269662921348312E-2</v>
       </c>
-      <c r="H44" s="26"/>
-      <c r="I44" s="26"/>
-      <c r="J44" s="26">
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19">
         <f>MAX(J4:J42)</f>
         <v>180</v>
       </c>
-      <c r="K44" s="26">
+      <c r="K44" s="19">
         <f>MAX(K4:K42)</f>
         <v>11</v>
       </c>
-      <c r="L44" s="26">
+      <c r="L44" s="19">
         <f>MAX(L4:L42)</f>
         <v>16</v>
       </c>
-      <c r="M44" s="27">
+      <c r="M44" s="20">
         <f>MAX(M4:M42)</f>
         <v>1</v>
       </c>
-      <c r="N44" s="28">
+      <c r="N44" s="21">
         <f>MAX(N4:N42)</f>
         <v>9.03954802259887E-2</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A45" s="29" t="s">
+      <c r="A45" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="30"/>
-      <c r="C45" s="31">
+      <c r="B45" s="23"/>
+      <c r="C45" s="24">
         <f>MIN(C4:C42)</f>
         <v>153</v>
       </c>
-      <c r="D45" s="31">
+      <c r="D45" s="24">
         <f>MIN(D4:D42)</f>
         <v>0</v>
       </c>
-      <c r="E45" s="31">
+      <c r="E45" s="24">
         <f>MIN(E4:E42)</f>
         <v>0</v>
       </c>
-      <c r="F45" s="32">
+      <c r="F45" s="25">
         <f>MIN(F4:F42)</f>
         <v>0.7</v>
       </c>
-      <c r="G45" s="32">
+      <c r="G45" s="25">
         <f>MIN(G4:G42)</f>
         <v>0</v>
       </c>
-      <c r="H45" s="31"/>
-      <c r="I45" s="31"/>
-      <c r="J45" s="31">
+      <c r="H45" s="24"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24">
         <f>MIN(J4:J42)</f>
         <v>169</v>
       </c>
-      <c r="K45" s="31">
+      <c r="K45" s="24">
         <f>MIN(K4:K42)</f>
         <v>0</v>
       </c>
-      <c r="L45" s="31">
+      <c r="L45" s="24">
         <f>MIN(L4:L42)</f>
         <v>0</v>
       </c>
-      <c r="M45" s="32">
+      <c r="M45" s="25">
         <f>MIN(M4:M42)</f>
         <v>0.87777777777777777</v>
       </c>
-      <c r="N45" s="33">
+      <c r="N45" s="26">
         <f>MIN(N4:N42)</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="34" t="s">
+      <c r="A46" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="35"/>
-      <c r="C46" s="36">
+      <c r="B46" s="28"/>
+      <c r="C46" s="29">
         <f>AVERAGE(C4:C42)</f>
         <v>176.25641025641025</v>
       </c>
-      <c r="D46" s="36">
+      <c r="D46" s="29">
         <f>AVERAGE(D4:D42)</f>
         <v>3.7435897435897436</v>
       </c>
-      <c r="E46" s="36">
+      <c r="E46" s="29">
         <f>AVERAGE(E4:E42)</f>
         <v>2.8974358974358974</v>
       </c>
-      <c r="F46" s="37">
+      <c r="F46" s="30">
         <f>AVERAGE(F4:F42)</f>
         <v>0.95840455840455829</v>
       </c>
-      <c r="G46" s="37">
+      <c r="G46" s="30">
         <f>AVERAGE(G4:G42)</f>
         <v>1.6450529467536674E-2</v>
       </c>
-      <c r="H46" s="38"/>
-      <c r="I46" s="38"/>
-      <c r="J46" s="36">
+      <c r="H46" s="31"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="29">
         <f>AVERAGE(J4:J42)</f>
         <v>176.84615384615384</v>
       </c>
-      <c r="K46" s="36">
+      <c r="K46" s="29">
         <f>AVERAGE(K4:K42)</f>
         <v>3.1538461538461537</v>
       </c>
-      <c r="L46" s="36">
+      <c r="L46" s="29">
         <f>AVERAGE(L4:L42)</f>
         <v>3.2820512820512819</v>
       </c>
-      <c r="M46" s="37">
+      <c r="M46" s="30">
         <f>AVERAGE(M4:M42)</f>
         <v>0.96495726495726453</v>
       </c>
-      <c r="N46" s="39">
+      <c r="N46" s="32">
         <f>AVERAGE(N4:N42)</f>
         <v>1.8553484810524122E-2</v>
       </c>

</xml_diff>